<commit_message>
Small Changes to Excel. Renamed illness to effect
</commit_message>
<xml_diff>
--- a/howtodoinjava_demo.xlsx
+++ b/howtodoinjava_demo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aug30\IdeaProjects\OregonTrail\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04FE447E-8E43-4B73-904D-606FBAB08728}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4C27FF8-B9F4-4F07-B713-11FFD18270BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-78" yWindow="0" windowWidth="7620" windowHeight="12318" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Stores" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
   <si>
     <t>Game Data Configuration Sheet</t>
   </si>
@@ -86,6 +86,9 @@
   </si>
   <si>
     <t>WATER</t>
+  </si>
+  <si>
+    <t>Number of items</t>
   </si>
 </sst>
 </file>
@@ -123,9 +126,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -443,7 +444,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -473,6 +474,12 @@
       <c r="A4" t="s">
         <v>1</v>
       </c>
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4">
+        <v>9</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
@@ -645,9 +652,6 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:F2"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Made Main Loop controlled and implemented stores into the main game
</commit_message>
<xml_diff>
--- a/howtodoinjava_demo.xlsx
+++ b/howtodoinjava_demo.xlsx
@@ -8,14 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aug30\IdeaProjects\OregonTrail\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4C27FF8-B9F4-4F07-B713-11FFD18270BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85F3A8F6-5930-449F-9169-8D8C4D83EFA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Stores" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -444,7 +457,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>